<commit_message>
update load file excel set on-off
</commit_message>
<xml_diff>
--- a/inverter_control/inverter_config.xlsx
+++ b/inverter_control/inverter_config.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -608,19 +608,19 @@
         <v>Zone B</v>
       </c>
       <c r="B11" t="str">
-        <v>B2</v>
+        <v>B3R1</v>
       </c>
       <c r="C11" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D11" t="str">
-        <v>10.10.10.110</v>
+        <v>10.10.10.121</v>
       </c>
       <c r="E11" t="str">
         <v>OK</v>
       </c>
       <c r="F11" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="12">
@@ -631,16 +631,16 @@
         <v>B3R1</v>
       </c>
       <c r="C12" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D12" t="str">
-        <v>10.10.10.121</v>
+        <v>10.10.10.122</v>
       </c>
       <c r="E12" t="str">
         <v>OK</v>
       </c>
       <c r="F12" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="13">
@@ -651,16 +651,16 @@
         <v>B3R1</v>
       </c>
       <c r="C13" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D13" t="str">
-        <v>10.10.10.122</v>
+        <v>10.10.10.123</v>
       </c>
       <c r="E13" t="str">
         <v>OK</v>
       </c>
       <c r="F13" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="14">
@@ -671,16 +671,16 @@
         <v>B3R1</v>
       </c>
       <c r="C14" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D14" t="str">
-        <v>10.10.10.123</v>
+        <v>10.10.10.124</v>
       </c>
       <c r="E14" t="str">
         <v>OK</v>
       </c>
       <c r="F14" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="15">
@@ -691,16 +691,16 @@
         <v>B3R1</v>
       </c>
       <c r="C15" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D15" t="str">
-        <v>10.10.10.124</v>
+        <v>10.10.10.125</v>
       </c>
       <c r="E15" t="str">
         <v>OK</v>
       </c>
       <c r="F15" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="16">
@@ -711,16 +711,16 @@
         <v>B3R1</v>
       </c>
       <c r="C16" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D16" t="str">
-        <v>10.10.10.125</v>
+        <v>10.10.10.126</v>
       </c>
       <c r="E16" t="str">
         <v>OK</v>
       </c>
       <c r="F16" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="17">
@@ -731,16 +731,16 @@
         <v>B3R1</v>
       </c>
       <c r="C17" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D17" t="str">
-        <v>10.10.10.126</v>
+        <v>10.10.10.127</v>
       </c>
       <c r="E17" t="str">
         <v>OK</v>
       </c>
       <c r="F17" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="18">
@@ -751,16 +751,16 @@
         <v>B3R1</v>
       </c>
       <c r="C18" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D18" t="str">
-        <v>10.10.10.127</v>
+        <v>10.10.10.128</v>
       </c>
       <c r="E18" t="str">
         <v>OK</v>
       </c>
       <c r="F18" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="19">
@@ -771,16 +771,16 @@
         <v>B3R1</v>
       </c>
       <c r="C19" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D19" t="str">
-        <v>10.10.10.128</v>
+        <v>10.10.10.129</v>
       </c>
       <c r="E19" t="str">
         <v>OK</v>
       </c>
       <c r="F19" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="20">
@@ -788,19 +788,19 @@
         <v>Zone B</v>
       </c>
       <c r="B20" t="str">
-        <v>B3R1</v>
+        <v>B3R2</v>
       </c>
       <c r="C20" t="str">
-        <v>INV-09</v>
+        <v>INV-01</v>
       </c>
       <c r="D20" t="str">
-        <v>10.10.10.129</v>
+        <v>10.10.10.111</v>
       </c>
       <c r="E20" t="str">
         <v>OK</v>
       </c>
       <c r="F20" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="21">
@@ -811,16 +811,16 @@
         <v>B3R2</v>
       </c>
       <c r="C21" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D21" t="str">
-        <v>10.10.10.111</v>
+        <v>10.10.10.112</v>
       </c>
       <c r="E21" t="str">
         <v>OK</v>
       </c>
       <c r="F21" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="22">
@@ -831,16 +831,16 @@
         <v>B3R2</v>
       </c>
       <c r="C22" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D22" t="str">
-        <v>10.10.10.112</v>
+        <v>10.10.10.113</v>
       </c>
       <c r="E22" t="str">
         <v>OK</v>
       </c>
       <c r="F22" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="23">
@@ -851,16 +851,16 @@
         <v>B3R2</v>
       </c>
       <c r="C23" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D23" t="str">
-        <v>10.10.10.113</v>
+        <v>10.10.10.114</v>
       </c>
       <c r="E23" t="str">
         <v>OK</v>
       </c>
       <c r="F23" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="24">
@@ -871,16 +871,16 @@
         <v>B3R2</v>
       </c>
       <c r="C24" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D24" t="str">
-        <v>10.10.10.114</v>
+        <v>10.10.10.115</v>
       </c>
       <c r="E24" t="str">
         <v>OK</v>
       </c>
       <c r="F24" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="25">
@@ -891,16 +891,16 @@
         <v>B3R2</v>
       </c>
       <c r="C25" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D25" t="str">
-        <v>10.10.10.115</v>
+        <v>10.10.10.116</v>
       </c>
       <c r="E25" t="str">
         <v>OK</v>
       </c>
       <c r="F25" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="26">
@@ -911,16 +911,16 @@
         <v>B3R2</v>
       </c>
       <c r="C26" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D26" t="str">
-        <v>10.10.10.116</v>
+        <v>10.10.10.117</v>
       </c>
       <c r="E26" t="str">
         <v>OK</v>
       </c>
       <c r="F26" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="27">
@@ -931,16 +931,16 @@
         <v>B3R2</v>
       </c>
       <c r="C27" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D27" t="str">
-        <v>10.10.10.117</v>
+        <v>10.10.10.118</v>
       </c>
       <c r="E27" t="str">
         <v>OK</v>
       </c>
       <c r="F27" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="28">
@@ -951,16 +951,16 @@
         <v>B3R2</v>
       </c>
       <c r="C28" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D28" t="str">
-        <v>10.10.10.118</v>
+        <v>10.10.10.119</v>
       </c>
       <c r="E28" t="str">
         <v>OK</v>
       </c>
       <c r="F28" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="29">
@@ -968,19 +968,19 @@
         <v>Zone B</v>
       </c>
       <c r="B29" t="str">
-        <v>B3R2</v>
+        <v>B4R1</v>
       </c>
       <c r="C29" t="str">
-        <v>INV-09</v>
+        <v>INV-01</v>
       </c>
       <c r="D29" t="str">
-        <v>10.10.10.119</v>
+        <v>10.10.10.141</v>
       </c>
       <c r="E29" t="str">
         <v>OK</v>
       </c>
       <c r="F29" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="30">
@@ -991,16 +991,16 @@
         <v>B4R1</v>
       </c>
       <c r="C30" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D30" t="str">
-        <v>10.10.10.141</v>
+        <v>10.10.10.142</v>
       </c>
       <c r="E30" t="str">
         <v>OK</v>
       </c>
       <c r="F30" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="31">
@@ -1011,16 +1011,16 @@
         <v>B4R1</v>
       </c>
       <c r="C31" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D31" t="str">
-        <v>10.10.10.142</v>
+        <v>10.10.10.143</v>
       </c>
       <c r="E31" t="str">
         <v>OK</v>
       </c>
       <c r="F31" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="32">
@@ -1031,16 +1031,16 @@
         <v>B4R1</v>
       </c>
       <c r="C32" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D32" t="str">
-        <v>10.10.10.143</v>
+        <v>10.10.10.144</v>
       </c>
       <c r="E32" t="str">
         <v>OK</v>
       </c>
       <c r="F32" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="33">
@@ -1051,16 +1051,16 @@
         <v>B4R1</v>
       </c>
       <c r="C33" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D33" t="str">
-        <v>10.10.10.144</v>
+        <v>10.10.10.145</v>
       </c>
       <c r="E33" t="str">
         <v>OK</v>
       </c>
       <c r="F33" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="34">
@@ -1071,16 +1071,16 @@
         <v>B4R1</v>
       </c>
       <c r="C34" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D34" t="str">
-        <v>10.10.10.145</v>
+        <v>10.10.10.146</v>
       </c>
       <c r="E34" t="str">
         <v>OK</v>
       </c>
       <c r="F34" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="35">
@@ -1091,16 +1091,16 @@
         <v>B4R1</v>
       </c>
       <c r="C35" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D35" t="str">
-        <v>10.10.10.146</v>
+        <v>10.10.10.147</v>
       </c>
       <c r="E35" t="str">
         <v>OK</v>
       </c>
       <c r="F35" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="36">
@@ -1111,16 +1111,16 @@
         <v>B4R1</v>
       </c>
       <c r="C36" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D36" t="str">
-        <v>10.10.10.147</v>
+        <v>10.10.10.148</v>
       </c>
       <c r="E36" t="str">
         <v>OK</v>
       </c>
       <c r="F36" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="37">
@@ -1131,16 +1131,16 @@
         <v>B4R1</v>
       </c>
       <c r="C37" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D37" t="str">
-        <v>10.10.10.148</v>
+        <v>10.10.10.149</v>
       </c>
       <c r="E37" t="str">
         <v>OK</v>
       </c>
       <c r="F37" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="38">
@@ -1151,16 +1151,16 @@
         <v>B4R1</v>
       </c>
       <c r="C38" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D38" t="str">
-        <v>10.10.10.149</v>
+        <v>10.10.10.150</v>
       </c>
       <c r="E38" t="str">
         <v>OK</v>
       </c>
       <c r="F38" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="39">
@@ -1168,19 +1168,19 @@
         <v>Zone B</v>
       </c>
       <c r="B39" t="str">
-        <v>B4R1</v>
+        <v>B4R2</v>
       </c>
       <c r="C39" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D39" t="str">
-        <v>10.10.10.150</v>
+        <v>10.10.10.131</v>
       </c>
       <c r="E39" t="str">
         <v>OK</v>
       </c>
       <c r="F39" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="40">
@@ -1191,16 +1191,16 @@
         <v>B4R2</v>
       </c>
       <c r="C40" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D40" t="str">
-        <v>10.10.10.131</v>
+        <v>10.10.10.132</v>
       </c>
       <c r="E40" t="str">
         <v>OK</v>
       </c>
       <c r="F40" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="41">
@@ -1211,16 +1211,16 @@
         <v>B4R2</v>
       </c>
       <c r="C41" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D41" t="str">
-        <v>10.10.10.132</v>
+        <v>10.10.10.133</v>
       </c>
       <c r="E41" t="str">
         <v>OK</v>
       </c>
       <c r="F41" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="42">
@@ -1231,16 +1231,16 @@
         <v>B4R2</v>
       </c>
       <c r="C42" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D42" t="str">
-        <v>10.10.10.133</v>
+        <v>10.10.10.134</v>
       </c>
       <c r="E42" t="str">
         <v>OK</v>
       </c>
       <c r="F42" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="43">
@@ -1251,16 +1251,16 @@
         <v>B4R2</v>
       </c>
       <c r="C43" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D43" t="str">
-        <v>10.10.10.134</v>
+        <v>10.10.10.135</v>
       </c>
       <c r="E43" t="str">
         <v>OK</v>
       </c>
       <c r="F43" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="44">
@@ -1271,16 +1271,16 @@
         <v>B4R2</v>
       </c>
       <c r="C44" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D44" t="str">
-        <v>10.10.10.135</v>
+        <v>10.10.10.136</v>
       </c>
       <c r="E44" t="str">
         <v>OK</v>
       </c>
       <c r="F44" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="45">
@@ -1291,16 +1291,16 @@
         <v>B4R2</v>
       </c>
       <c r="C45" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D45" t="str">
-        <v>10.10.10.136</v>
+        <v>10.10.10.137</v>
       </c>
       <c r="E45" t="str">
         <v>OK</v>
       </c>
       <c r="F45" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="46">
@@ -1311,16 +1311,16 @@
         <v>B4R2</v>
       </c>
       <c r="C46" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D46" t="str">
-        <v>10.10.10.137</v>
+        <v>10.10.10.138</v>
       </c>
       <c r="E46" t="str">
         <v>OK</v>
       </c>
       <c r="F46" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="47">
@@ -1331,16 +1331,16 @@
         <v>B4R2</v>
       </c>
       <c r="C47" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D47" t="str">
-        <v>10.10.10.138</v>
+        <v>10.10.10.139</v>
       </c>
       <c r="E47" t="str">
         <v>OK</v>
       </c>
       <c r="F47" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="48">
@@ -1351,16 +1351,16 @@
         <v>B4R2</v>
       </c>
       <c r="C48" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D48" t="str">
-        <v>10.10.10.139</v>
+        <v>10.10.10.140</v>
       </c>
       <c r="E48" t="str">
         <v>OK</v>
       </c>
       <c r="F48" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="49">
@@ -1368,19 +1368,19 @@
         <v>Zone B</v>
       </c>
       <c r="B49" t="str">
-        <v>B4R2</v>
+        <v>B5R1</v>
       </c>
       <c r="C49" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D49" t="str">
-        <v>10.10.10.140</v>
+        <v>10.10.10.161</v>
       </c>
       <c r="E49" t="str">
         <v>OK</v>
       </c>
       <c r="F49" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="50">
@@ -1391,16 +1391,16 @@
         <v>B5R1</v>
       </c>
       <c r="C50" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D50" t="str">
-        <v>10.10.10.161</v>
+        <v>10.10.10.162</v>
       </c>
       <c r="E50" t="str">
         <v>OK</v>
       </c>
       <c r="F50" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="51">
@@ -1411,16 +1411,16 @@
         <v>B5R1</v>
       </c>
       <c r="C51" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D51" t="str">
-        <v>10.10.10.162</v>
+        <v>10.10.10.163</v>
       </c>
       <c r="E51" t="str">
         <v>OK</v>
       </c>
       <c r="F51" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="52">
@@ -1431,16 +1431,16 @@
         <v>B5R1</v>
       </c>
       <c r="C52" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D52" t="str">
-        <v>10.10.10.163</v>
+        <v>10.10.10.164</v>
       </c>
       <c r="E52" t="str">
         <v>OK</v>
       </c>
       <c r="F52" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="53">
@@ -1451,16 +1451,16 @@
         <v>B5R1</v>
       </c>
       <c r="C53" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D53" t="str">
-        <v>10.10.10.164</v>
+        <v>10.10.10.165</v>
       </c>
       <c r="E53" t="str">
         <v>OK</v>
       </c>
       <c r="F53" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="54">
@@ -1471,16 +1471,16 @@
         <v>B5R1</v>
       </c>
       <c r="C54" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D54" t="str">
-        <v>10.10.10.165</v>
+        <v>10.10.10.166</v>
       </c>
       <c r="E54" t="str">
         <v>OK</v>
       </c>
       <c r="F54" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="55">
@@ -1491,16 +1491,16 @@
         <v>B5R1</v>
       </c>
       <c r="C55" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D55" t="str">
-        <v>10.10.10.166</v>
+        <v>10.10.10.167</v>
       </c>
       <c r="E55" t="str">
         <v>OK</v>
       </c>
       <c r="F55" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="56">
@@ -1511,16 +1511,16 @@
         <v>B5R1</v>
       </c>
       <c r="C56" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D56" t="str">
-        <v>10.10.10.167</v>
+        <v>10.10.10.168</v>
       </c>
       <c r="E56" t="str">
         <v>OK</v>
       </c>
       <c r="F56" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="57">
@@ -1531,16 +1531,16 @@
         <v>B5R1</v>
       </c>
       <c r="C57" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D57" t="str">
-        <v>10.10.10.168</v>
+        <v>10.10.10.169</v>
       </c>
       <c r="E57" t="str">
         <v>OK</v>
       </c>
       <c r="F57" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="58">
@@ -1551,16 +1551,16 @@
         <v>B5R1</v>
       </c>
       <c r="C58" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D58" t="str">
-        <v>10.10.10.169</v>
+        <v>10.10.10.170</v>
       </c>
       <c r="E58" t="str">
         <v>OK</v>
       </c>
       <c r="F58" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="59">
@@ -1568,19 +1568,19 @@
         <v>Zone B</v>
       </c>
       <c r="B59" t="str">
-        <v>B5R1</v>
+        <v>B5R2</v>
       </c>
       <c r="C59" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D59" t="str">
-        <v>10.10.10.170</v>
+        <v>10.10.10.151</v>
       </c>
       <c r="E59" t="str">
         <v>OK</v>
       </c>
       <c r="F59" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="60">
@@ -1591,16 +1591,16 @@
         <v>B5R2</v>
       </c>
       <c r="C60" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D60" t="str">
-        <v>10.10.10.151</v>
+        <v>10.10.10.152</v>
       </c>
       <c r="E60" t="str">
         <v>OK</v>
       </c>
       <c r="F60" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="61">
@@ -1611,16 +1611,16 @@
         <v>B5R2</v>
       </c>
       <c r="C61" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D61" t="str">
-        <v>10.10.10.152</v>
+        <v>10.10.10.153</v>
       </c>
       <c r="E61" t="str">
         <v>OK</v>
       </c>
       <c r="F61" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="62">
@@ -1631,16 +1631,16 @@
         <v>B5R2</v>
       </c>
       <c r="C62" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D62" t="str">
-        <v>10.10.10.153</v>
+        <v>10.10.10.154</v>
       </c>
       <c r="E62" t="str">
         <v>OK</v>
       </c>
       <c r="F62" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="63">
@@ -1651,16 +1651,16 @@
         <v>B5R2</v>
       </c>
       <c r="C63" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D63" t="str">
-        <v>10.10.10.154</v>
+        <v>10.10.10.155</v>
       </c>
       <c r="E63" t="str">
         <v>OK</v>
       </c>
       <c r="F63" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="64">
@@ -1671,16 +1671,16 @@
         <v>B5R2</v>
       </c>
       <c r="C64" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D64" t="str">
-        <v>10.10.10.155</v>
+        <v>10.10.10.156</v>
       </c>
       <c r="E64" t="str">
         <v>OK</v>
       </c>
       <c r="F64" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="65">
@@ -1691,16 +1691,16 @@
         <v>B5R2</v>
       </c>
       <c r="C65" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D65" t="str">
-        <v>10.10.10.156</v>
+        <v>10.10.10.157</v>
       </c>
       <c r="E65" t="str">
         <v>OK</v>
       </c>
       <c r="F65" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="66">
@@ -1711,16 +1711,16 @@
         <v>B5R2</v>
       </c>
       <c r="C66" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D66" t="str">
-        <v>10.10.10.157</v>
+        <v>10.10.10.158</v>
       </c>
       <c r="E66" t="str">
         <v>OK</v>
       </c>
       <c r="F66" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="67">
@@ -1731,16 +1731,16 @@
         <v>B5R2</v>
       </c>
       <c r="C67" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D67" t="str">
-        <v>10.10.10.158</v>
+        <v>10.10.10.159</v>
       </c>
       <c r="E67" t="str">
         <v>OK</v>
       </c>
       <c r="F67" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="68">
@@ -1751,16 +1751,16 @@
         <v>B5R2</v>
       </c>
       <c r="C68" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D68" t="str">
-        <v>10.10.10.159</v>
+        <v>10.10.10.160</v>
       </c>
       <c r="E68" t="str">
         <v>OK</v>
       </c>
       <c r="F68" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="69">
@@ -1768,19 +1768,19 @@
         <v>Zone B</v>
       </c>
       <c r="B69" t="str">
-        <v>B5R2</v>
+        <v>B6R1</v>
       </c>
       <c r="C69" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D69" t="str">
-        <v>10.10.10.160</v>
+        <v>10.10.10.181</v>
       </c>
       <c r="E69" t="str">
         <v>OK</v>
       </c>
       <c r="F69" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="70">
@@ -1791,16 +1791,16 @@
         <v>B6R1</v>
       </c>
       <c r="C70" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D70" t="str">
-        <v>10.10.10.181</v>
+        <v>10.10.10.182</v>
       </c>
       <c r="E70" t="str">
         <v>OK</v>
       </c>
       <c r="F70" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="71">
@@ -1811,16 +1811,16 @@
         <v>B6R1</v>
       </c>
       <c r="C71" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D71" t="str">
-        <v>10.10.10.182</v>
+        <v>10.10.10.183</v>
       </c>
       <c r="E71" t="str">
         <v>OK</v>
       </c>
       <c r="F71" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="72">
@@ -1831,16 +1831,16 @@
         <v>B6R1</v>
       </c>
       <c r="C72" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D72" t="str">
-        <v>10.10.10.183</v>
+        <v>10.10.10.184</v>
       </c>
       <c r="E72" t="str">
         <v>OK</v>
       </c>
       <c r="F72" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="73">
@@ -1851,16 +1851,16 @@
         <v>B6R1</v>
       </c>
       <c r="C73" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D73" t="str">
-        <v>10.10.10.184</v>
+        <v>10.10.10.185</v>
       </c>
       <c r="E73" t="str">
         <v>OK</v>
       </c>
       <c r="F73" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="74">
@@ -1871,16 +1871,16 @@
         <v>B6R1</v>
       </c>
       <c r="C74" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D74" t="str">
-        <v>10.10.10.185</v>
+        <v>10.10.10.186</v>
       </c>
       <c r="E74" t="str">
         <v>OK</v>
       </c>
       <c r="F74" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="75">
@@ -1891,16 +1891,16 @@
         <v>B6R1</v>
       </c>
       <c r="C75" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D75" t="str">
-        <v>10.10.10.186</v>
+        <v>10.10.10.187</v>
       </c>
       <c r="E75" t="str">
         <v>OK</v>
       </c>
       <c r="F75" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="76">
@@ -1911,16 +1911,16 @@
         <v>B6R1</v>
       </c>
       <c r="C76" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D76" t="str">
-        <v>10.10.10.187</v>
+        <v>10.10.10.188</v>
       </c>
       <c r="E76" t="str">
         <v>OK</v>
       </c>
       <c r="F76" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="77">
@@ -1931,16 +1931,16 @@
         <v>B6R1</v>
       </c>
       <c r="C77" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D77" t="str">
-        <v>10.10.10.188</v>
+        <v>10.10.10.189</v>
       </c>
       <c r="E77" t="str">
         <v>OK</v>
       </c>
       <c r="F77" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="78">
@@ -1951,16 +1951,16 @@
         <v>B6R1</v>
       </c>
       <c r="C78" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D78" t="str">
-        <v>10.10.10.189</v>
+        <v>10.10.10.190</v>
       </c>
       <c r="E78" t="str">
         <v>OK</v>
       </c>
       <c r="F78" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="79">
@@ -1968,19 +1968,19 @@
         <v>Zone B</v>
       </c>
       <c r="B79" t="str">
-        <v>B6R1</v>
+        <v>B6R2</v>
       </c>
       <c r="C79" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D79" t="str">
-        <v>10.10.10.190</v>
+        <v>10.10.10.171</v>
       </c>
       <c r="E79" t="str">
         <v>OK</v>
       </c>
       <c r="F79" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="80">
@@ -1991,16 +1991,16 @@
         <v>B6R2</v>
       </c>
       <c r="C80" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D80" t="str">
-        <v>10.10.10.171</v>
+        <v>10.10.10.172</v>
       </c>
       <c r="E80" t="str">
         <v>OK</v>
       </c>
       <c r="F80" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="81">
@@ -2011,16 +2011,16 @@
         <v>B6R2</v>
       </c>
       <c r="C81" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D81" t="str">
-        <v>10.10.10.172</v>
+        <v>10.10.10.173</v>
       </c>
       <c r="E81" t="str">
         <v>OK</v>
       </c>
       <c r="F81" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="82">
@@ -2031,16 +2031,16 @@
         <v>B6R2</v>
       </c>
       <c r="C82" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D82" t="str">
-        <v>10.10.10.173</v>
+        <v>10.10.10.174</v>
       </c>
       <c r="E82" t="str">
         <v>OK</v>
       </c>
       <c r="F82" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="83">
@@ -2051,16 +2051,16 @@
         <v>B6R2</v>
       </c>
       <c r="C83" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D83" t="str">
-        <v>10.10.10.174</v>
+        <v>10.10.10.175</v>
       </c>
       <c r="E83" t="str">
         <v>OK</v>
       </c>
       <c r="F83" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="84">
@@ -2071,16 +2071,16 @@
         <v>B6R2</v>
       </c>
       <c r="C84" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D84" t="str">
-        <v>10.10.10.175</v>
+        <v>10.10.10.176</v>
       </c>
       <c r="E84" t="str">
         <v>OK</v>
       </c>
       <c r="F84" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="85">
@@ -2091,16 +2091,16 @@
         <v>B6R2</v>
       </c>
       <c r="C85" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D85" t="str">
-        <v>10.10.10.176</v>
+        <v>10.10.10.177</v>
       </c>
       <c r="E85" t="str">
         <v>OK</v>
       </c>
       <c r="F85" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="86">
@@ -2111,16 +2111,16 @@
         <v>B6R2</v>
       </c>
       <c r="C86" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D86" t="str">
-        <v>10.10.10.177</v>
+        <v>10.10.10.178</v>
       </c>
       <c r="E86" t="str">
         <v>OK</v>
       </c>
       <c r="F86" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="87">
@@ -2131,16 +2131,16 @@
         <v>B6R2</v>
       </c>
       <c r="C87" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D87" t="str">
-        <v>10.10.10.178</v>
+        <v>10.10.10.179</v>
       </c>
       <c r="E87" t="str">
         <v>OK</v>
       </c>
       <c r="F87" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="88">
@@ -2151,16 +2151,16 @@
         <v>B6R2</v>
       </c>
       <c r="C88" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D88" t="str">
-        <v>10.10.10.179</v>
+        <v>10.10.10.180</v>
       </c>
       <c r="E88" t="str">
         <v>OK</v>
       </c>
       <c r="F88" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="89">
@@ -2168,19 +2168,19 @@
         <v>Zone B</v>
       </c>
       <c r="B89" t="str">
-        <v>B6R2</v>
+        <v>B7</v>
       </c>
       <c r="C89" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D89" t="str">
-        <v>10.10.10.180</v>
+        <v>10.10.10.191</v>
       </c>
       <c r="E89" t="str">
         <v>OK</v>
       </c>
       <c r="F89" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="90">
@@ -2191,16 +2191,16 @@
         <v>B7</v>
       </c>
       <c r="C90" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D90" t="str">
-        <v>10.10.10.191</v>
+        <v>10.10.10.192</v>
       </c>
       <c r="E90" t="str">
         <v>OK</v>
       </c>
       <c r="F90" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="91">
@@ -2211,16 +2211,16 @@
         <v>B7</v>
       </c>
       <c r="C91" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D91" t="str">
-        <v>10.10.10.192</v>
+        <v>10.10.10.193</v>
       </c>
       <c r="E91" t="str">
         <v>OK</v>
       </c>
       <c r="F91" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="92">
@@ -2231,16 +2231,16 @@
         <v>B7</v>
       </c>
       <c r="C92" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D92" t="str">
-        <v>10.10.10.193</v>
+        <v>10.10.10.194</v>
       </c>
       <c r="E92" t="str">
         <v>OK</v>
       </c>
       <c r="F92" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="93">
@@ -2251,16 +2251,16 @@
         <v>B7</v>
       </c>
       <c r="C93" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D93" t="str">
-        <v>10.10.10.194</v>
+        <v>10.10.10.195</v>
       </c>
       <c r="E93" t="str">
         <v>OK</v>
       </c>
       <c r="F93" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="94">
@@ -2271,16 +2271,16 @@
         <v>B7</v>
       </c>
       <c r="C94" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D94" t="str">
-        <v>10.10.10.195</v>
+        <v>10.10.10.196</v>
       </c>
       <c r="E94" t="str">
         <v>OK</v>
       </c>
       <c r="F94" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="95">
@@ -2291,16 +2291,16 @@
         <v>B7</v>
       </c>
       <c r="C95" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D95" t="str">
-        <v>10.10.10.196</v>
+        <v>10.10.10.197</v>
       </c>
       <c r="E95" t="str">
         <v>OK</v>
       </c>
       <c r="F95" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="96">
@@ -2311,16 +2311,16 @@
         <v>B7</v>
       </c>
       <c r="C96" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D96" t="str">
-        <v>10.10.10.197</v>
+        <v>10.10.10.198</v>
       </c>
       <c r="E96" t="str">
         <v>OK</v>
       </c>
       <c r="F96" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="97">
@@ -2331,16 +2331,16 @@
         <v>B7</v>
       </c>
       <c r="C97" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D97" t="str">
-        <v>10.10.10.198</v>
+        <v>10.10.10.199</v>
       </c>
       <c r="E97" t="str">
         <v>OK</v>
       </c>
       <c r="F97" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="98">
@@ -2351,16 +2351,16 @@
         <v>B7</v>
       </c>
       <c r="C98" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D98" t="str">
-        <v>10.10.10.199</v>
+        <v>10.10.10.200</v>
       </c>
       <c r="E98" t="str">
         <v>OK</v>
       </c>
       <c r="F98" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="99">
@@ -2368,19 +2368,19 @@
         <v>Zone B</v>
       </c>
       <c r="B99" t="str">
-        <v>B7</v>
+        <v>B8</v>
       </c>
       <c r="C99" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D99" t="str">
-        <v>10.10.10.200</v>
+        <v>10.10.10.201</v>
       </c>
       <c r="E99" t="str">
         <v>OK</v>
       </c>
       <c r="F99" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="100">
@@ -2391,16 +2391,16 @@
         <v>B8</v>
       </c>
       <c r="C100" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D100" t="str">
-        <v>10.10.10.201</v>
+        <v>10.10.10.202</v>
       </c>
       <c r="E100" t="str">
         <v>OK</v>
       </c>
       <c r="F100" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="101">
@@ -2411,16 +2411,16 @@
         <v>B8</v>
       </c>
       <c r="C101" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D101" t="str">
-        <v>10.10.10.202</v>
+        <v>10.10.10.203</v>
       </c>
       <c r="E101" t="str">
         <v>OK</v>
       </c>
       <c r="F101" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="102">
@@ -2431,16 +2431,16 @@
         <v>B8</v>
       </c>
       <c r="C102" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D102" t="str">
-        <v>10.10.10.203</v>
+        <v>10.10.10.204</v>
       </c>
       <c r="E102" t="str">
         <v>OK</v>
       </c>
       <c r="F102" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="103">
@@ -2451,16 +2451,16 @@
         <v>B8</v>
       </c>
       <c r="C103" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D103" t="str">
-        <v>10.10.10.204</v>
+        <v>10.10.10.205</v>
       </c>
       <c r="E103" t="str">
         <v>OK</v>
       </c>
       <c r="F103" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="104">
@@ -2468,19 +2468,19 @@
         <v>Zone B</v>
       </c>
       <c r="B104" t="str">
-        <v>B8</v>
+        <v>B11</v>
       </c>
       <c r="C104" t="str">
-        <v>INV-05</v>
+        <v>INV-01</v>
       </c>
       <c r="D104" t="str">
-        <v>10.10.10.205</v>
+        <v>10.10.10.211</v>
       </c>
       <c r="E104" t="str">
         <v>OK</v>
       </c>
       <c r="F104" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="105">
@@ -2491,16 +2491,16 @@
         <v>B11</v>
       </c>
       <c r="C105" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D105" t="str">
-        <v>10.10.10.211</v>
+        <v>10.10.10.212</v>
       </c>
       <c r="E105" t="str">
         <v>OK</v>
       </c>
       <c r="F105" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="106">
@@ -2511,16 +2511,16 @@
         <v>B11</v>
       </c>
       <c r="C106" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D106" t="str">
-        <v>10.10.10.212</v>
+        <v>10.10.10.213</v>
       </c>
       <c r="E106" t="str">
         <v>OK</v>
       </c>
       <c r="F106" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="107">
@@ -2531,16 +2531,16 @@
         <v>B11</v>
       </c>
       <c r="C107" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D107" t="str">
-        <v>10.10.10.213</v>
+        <v>10.10.10.214</v>
       </c>
       <c r="E107" t="str">
         <v>OK</v>
       </c>
       <c r="F107" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="108">
@@ -2551,16 +2551,16 @@
         <v>B11</v>
       </c>
       <c r="C108" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D108" t="str">
-        <v>10.10.10.214</v>
+        <v>10.10.10.215</v>
       </c>
       <c r="E108" t="str">
         <v>OK</v>
       </c>
       <c r="F108" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="109">
@@ -2571,16 +2571,16 @@
         <v>B11</v>
       </c>
       <c r="C109" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D109" t="str">
-        <v>10.10.10.215</v>
+        <v>10.10.10.216</v>
       </c>
       <c r="E109" t="str">
         <v>OK</v>
       </c>
       <c r="F109" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="110">
@@ -2591,16 +2591,16 @@
         <v>B11</v>
       </c>
       <c r="C110" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D110" t="str">
-        <v>10.10.10.216</v>
+        <v>10.10.10.217</v>
       </c>
       <c r="E110" t="str">
         <v>OK</v>
       </c>
       <c r="F110" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="111">
@@ -2611,16 +2611,16 @@
         <v>B11</v>
       </c>
       <c r="C111" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D111" t="str">
-        <v>10.10.10.217</v>
+        <v>10.10.10.218</v>
       </c>
       <c r="E111" t="str">
         <v>OK</v>
       </c>
       <c r="F111" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="112">
@@ -2631,16 +2631,16 @@
         <v>B11</v>
       </c>
       <c r="C112" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D112" t="str">
-        <v>10.10.10.218</v>
+        <v>10.10.10.219</v>
       </c>
       <c r="E112" t="str">
         <v>OK</v>
       </c>
       <c r="F112" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="113">
@@ -2651,16 +2651,16 @@
         <v>B11</v>
       </c>
       <c r="C113" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D113" t="str">
-        <v>10.10.10.219</v>
+        <v>10.10.10.220</v>
       </c>
       <c r="E113" t="str">
         <v>OK</v>
       </c>
       <c r="F113" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="114">
@@ -2668,19 +2668,19 @@
         <v>Zone B</v>
       </c>
       <c r="B114" t="str">
-        <v>B11</v>
+        <v>B12</v>
       </c>
       <c r="C114" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D114" t="str">
-        <v>10.10.10.220</v>
+        <v>10.10.10.241</v>
       </c>
       <c r="E114" t="str">
         <v>OK</v>
       </c>
       <c r="F114" t="str">
-        <v>Inverter số 10</v>
+        <v>Inverter số 1</v>
       </c>
     </row>
     <row r="115">
@@ -2691,16 +2691,16 @@
         <v>B12</v>
       </c>
       <c r="C115" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D115" t="str">
-        <v>10.10.10.241</v>
+        <v>10.10.10.242</v>
       </c>
       <c r="E115" t="str">
         <v>OK</v>
       </c>
       <c r="F115" t="str">
-        <v>Inverter số 1</v>
+        <v>Inverter số 2</v>
       </c>
     </row>
     <row r="116">
@@ -2711,16 +2711,16 @@
         <v>B12</v>
       </c>
       <c r="C116" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D116" t="str">
-        <v>10.10.10.242</v>
+        <v>10.10.10.243</v>
       </c>
       <c r="E116" t="str">
         <v>OK</v>
       </c>
       <c r="F116" t="str">
-        <v>Inverter số 2</v>
+        <v>Inverter số 3</v>
       </c>
     </row>
     <row r="117">
@@ -2731,16 +2731,16 @@
         <v>B12</v>
       </c>
       <c r="C117" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D117" t="str">
-        <v>10.10.10.243</v>
+        <v>10.10.10.244</v>
       </c>
       <c r="E117" t="str">
         <v>OK</v>
       </c>
       <c r="F117" t="str">
-        <v>Inverter số 3</v>
+        <v>Inverter số 4</v>
       </c>
     </row>
     <row r="118">
@@ -2751,16 +2751,16 @@
         <v>B12</v>
       </c>
       <c r="C118" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D118" t="str">
-        <v>10.10.10.244</v>
+        <v>10.10.10.245</v>
       </c>
       <c r="E118" t="str">
         <v>OK</v>
       </c>
       <c r="F118" t="str">
-        <v>Inverter số 4</v>
+        <v>Inverter số 5</v>
       </c>
     </row>
     <row r="119">
@@ -2771,16 +2771,16 @@
         <v>B12</v>
       </c>
       <c r="C119" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D119" t="str">
-        <v>10.10.10.245</v>
+        <v>10.10.10.246</v>
       </c>
       <c r="E119" t="str">
         <v>OK</v>
       </c>
       <c r="F119" t="str">
-        <v>Inverter số 5</v>
+        <v>Inverter số 6</v>
       </c>
     </row>
     <row r="120">
@@ -2791,16 +2791,16 @@
         <v>B12</v>
       </c>
       <c r="C120" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D120" t="str">
-        <v>10.10.10.246</v>
+        <v>10.10.10.247</v>
       </c>
       <c r="E120" t="str">
         <v>OK</v>
       </c>
       <c r="F120" t="str">
-        <v>Inverter số 6</v>
+        <v>Inverter số 7</v>
       </c>
     </row>
     <row r="121">
@@ -2811,16 +2811,16 @@
         <v>B12</v>
       </c>
       <c r="C121" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D121" t="str">
-        <v>10.10.10.247</v>
+        <v>10.10.10.248</v>
       </c>
       <c r="E121" t="str">
         <v>OK</v>
       </c>
       <c r="F121" t="str">
-        <v>Inverter số 7</v>
+        <v>Inverter số 8</v>
       </c>
     </row>
     <row r="122">
@@ -2831,16 +2831,16 @@
         <v>B12</v>
       </c>
       <c r="C122" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D122" t="str">
-        <v>10.10.10.248</v>
+        <v>10.10.10.249</v>
       </c>
       <c r="E122" t="str">
         <v>OK</v>
       </c>
       <c r="F122" t="str">
-        <v>Inverter số 8</v>
+        <v>Inverter số 9</v>
       </c>
     </row>
     <row r="123">
@@ -2851,16 +2851,16 @@
         <v>B12</v>
       </c>
       <c r="C123" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D123" t="str">
-        <v>10.10.10.249</v>
+        <v>10.10.10.250</v>
       </c>
       <c r="E123" t="str">
         <v>OK</v>
       </c>
       <c r="F123" t="str">
-        <v>Inverter số 9</v>
+        <v>Inverter số 10</v>
       </c>
     </row>
     <row r="124">
@@ -2868,19 +2868,19 @@
         <v>Zone B</v>
       </c>
       <c r="B124" t="str">
-        <v>B12</v>
+        <v>B13-14</v>
       </c>
       <c r="C124" t="str">
-        <v>INV-10</v>
+        <v>INV-01</v>
       </c>
       <c r="D124" t="str">
-        <v>10.10.10.250</v>
+        <v>10.10.10.221</v>
       </c>
       <c r="E124" t="str">
         <v>OK</v>
       </c>
       <c r="F124" t="str">
-        <v>Inverter số 10</v>
+        <v>B13 Inverter số 1</v>
       </c>
     </row>
     <row r="125">
@@ -2891,16 +2891,16 @@
         <v>B13-14</v>
       </c>
       <c r="C125" t="str">
-        <v>INV-01</v>
+        <v>INV-02</v>
       </c>
       <c r="D125" t="str">
-        <v>10.10.10.221</v>
+        <v>10.10.10.222</v>
       </c>
       <c r="E125" t="str">
         <v>OK</v>
       </c>
       <c r="F125" t="str">
-        <v>B13 Inverter số 1</v>
+        <v>B13 Inverter số 2</v>
       </c>
     </row>
     <row r="126">
@@ -2911,16 +2911,16 @@
         <v>B13-14</v>
       </c>
       <c r="C126" t="str">
-        <v>INV-02</v>
+        <v>INV-03</v>
       </c>
       <c r="D126" t="str">
-        <v>10.10.10.222</v>
+        <v>10.10.10.223</v>
       </c>
       <c r="E126" t="str">
         <v>OK</v>
       </c>
       <c r="F126" t="str">
-        <v>B13 Inverter số 2</v>
+        <v>B13 Inverter số 3</v>
       </c>
     </row>
     <row r="127">
@@ -2931,16 +2931,16 @@
         <v>B13-14</v>
       </c>
       <c r="C127" t="str">
-        <v>INV-03</v>
+        <v>INV-04</v>
       </c>
       <c r="D127" t="str">
-        <v>10.10.10.223</v>
+        <v>10.10.10.224</v>
       </c>
       <c r="E127" t="str">
         <v>OK</v>
       </c>
       <c r="F127" t="str">
-        <v>B13 Inverter số 3</v>
+        <v>B13 Inverter số 4</v>
       </c>
     </row>
     <row r="128">
@@ -2951,16 +2951,16 @@
         <v>B13-14</v>
       </c>
       <c r="C128" t="str">
-        <v>INV-04</v>
+        <v>INV-05</v>
       </c>
       <c r="D128" t="str">
-        <v>10.10.10.224</v>
+        <v>10.10.10.225</v>
       </c>
       <c r="E128" t="str">
         <v>OK</v>
       </c>
       <c r="F128" t="str">
-        <v>B13 Inverter số 4</v>
+        <v>B13 Inverter số 5</v>
       </c>
     </row>
     <row r="129">
@@ -2971,16 +2971,16 @@
         <v>B13-14</v>
       </c>
       <c r="C129" t="str">
-        <v>INV-05</v>
+        <v>INV-06</v>
       </c>
       <c r="D129" t="str">
-        <v>10.10.10.225</v>
+        <v>10.10.10.226</v>
       </c>
       <c r="E129" t="str">
         <v>OK</v>
       </c>
       <c r="F129" t="str">
-        <v>B13 Inverter số 5</v>
+        <v>B13 Inverter số 6</v>
       </c>
     </row>
     <row r="130">
@@ -2991,16 +2991,16 @@
         <v>B13-14</v>
       </c>
       <c r="C130" t="str">
-        <v>INV-06</v>
+        <v>INV-07</v>
       </c>
       <c r="D130" t="str">
-        <v>10.10.10.226</v>
+        <v>10.10.10.231</v>
       </c>
       <c r="E130" t="str">
         <v>OK</v>
       </c>
       <c r="F130" t="str">
-        <v>B13 Inverter số 6</v>
+        <v>B14 Inverter số 1</v>
       </c>
     </row>
     <row r="131">
@@ -3011,16 +3011,16 @@
         <v>B13-14</v>
       </c>
       <c r="C131" t="str">
-        <v>INV-07</v>
+        <v>INV-08</v>
       </c>
       <c r="D131" t="str">
-        <v>10.10.10.231</v>
+        <v>10.10.10.232</v>
       </c>
       <c r="E131" t="str">
         <v>OK</v>
       </c>
       <c r="F131" t="str">
-        <v>B14 Inverter số 1</v>
+        <v>B14 Inverter số 2</v>
       </c>
     </row>
     <row r="132">
@@ -3031,16 +3031,16 @@
         <v>B13-14</v>
       </c>
       <c r="C132" t="str">
-        <v>INV-08</v>
+        <v>INV-09</v>
       </c>
       <c r="D132" t="str">
-        <v>10.10.10.232</v>
+        <v>10.10.10.233</v>
       </c>
       <c r="E132" t="str">
         <v>OK</v>
       </c>
       <c r="F132" t="str">
-        <v>B14 Inverter số 2</v>
+        <v>B14 Inverter số 3</v>
       </c>
     </row>
     <row r="133">
@@ -3051,41 +3051,21 @@
         <v>B13-14</v>
       </c>
       <c r="C133" t="str">
-        <v>INV-09</v>
+        <v>INV-10</v>
       </c>
       <c r="D133" t="str">
-        <v>10.10.10.233</v>
+        <v>10.10.10.234</v>
       </c>
       <c r="E133" t="str">
         <v>OK</v>
       </c>
       <c r="F133" t="str">
-        <v>B14 Inverter số 3</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="str">
-        <v>Zone B</v>
-      </c>
-      <c r="B134" t="str">
-        <v>B13-14</v>
-      </c>
-      <c r="C134" t="str">
-        <v>INV-10</v>
-      </c>
-      <c r="D134" t="str">
-        <v>10.10.10.234</v>
-      </c>
-      <c r="E134" t="str">
-        <v>OK</v>
-      </c>
-      <c r="F134" t="str">
         <v>B14 Inverter số 4</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F134"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F133"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3116,7 +3096,7 @@
         <v>OFF</v>
       </c>
       <c r="C2" t="str">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -3127,7 +3107,7 @@
         <v>OFF</v>
       </c>
       <c r="C3" t="str">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -3138,7 +3118,7 @@
         <v>OFF</v>
       </c>
       <c r="C4" t="str">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -3149,7 +3129,7 @@
         <v>OFF</v>
       </c>
       <c r="C5" t="str">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -3160,7 +3140,7 @@
         <v>ON</v>
       </c>
       <c r="C6" t="str">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -3171,7 +3151,7 @@
         <v>ON</v>
       </c>
       <c r="C7" t="str">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -3182,7 +3162,7 @@
         <v>ON</v>
       </c>
       <c r="C8" t="str">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">

</xml_diff>